<commit_message>
Had not updated the branch properly. I have also commented out the code for connecting to my dropbox
</commit_message>
<xml_diff>
--- a/data/describe/LessonTree.xlsx
+++ b/data/describe/LessonTree.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4FC9BD-37F3-4326-BF56-21857B678890}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8DDCE0-052E-47A8-BA3D-1F8B078FDEFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,7 +569,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -656,6 +656,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1790,10 +1793,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -2162,6 +2165,9 @@
         <v>64</v>
       </c>
     </row>
+    <row r="22" spans="1:5" ht="19.899999999999999" customHeight="1">
+      <c r="C22" s="29"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>